<commit_message>
mensaje de asignacion del cliente
</commit_message>
<xml_diff>
--- a/public/import-excel-invoices/caproin-import-invoices.xlsx
+++ b/public/import-excel-invoices/caproin-import-invoices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">Número de Factura</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">Comentarios u observaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rbrekke@example.org</t>
   </si>
   <si>
     <t xml:space="preserve">Observaciones</t>
@@ -187,11 +190,11 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.67"/>
@@ -202,11 +205,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.2"/>
   </cols>
   <sheetData>
@@ -279,8 +282,8 @@
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>150000000</v>
@@ -307,12 +310,64 @@
         <v>43308</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>8575529522</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>63909844</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1222020</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>150000000</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>123123</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>100000</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="rbrekke@example.org"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Añadido tipo de pago
</commit_message>
<xml_diff>
--- a/public/import-excel-invoices/caproin-import-invoices.xlsx
+++ b/public/import-excel-invoices/caproin-import-invoices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">Número de Factura</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de pago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor Pagado</t>
   </si>
   <si>
     <t xml:space="preserve">Valor</t>
@@ -188,13 +194,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1048576"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.67"/>
@@ -202,18 +208,18 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="17.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="32.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="34.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="25.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="26.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -261,6 +267,12 @@
       </c>
       <c r="P1" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,34 +295,40 @@
         <v>1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>150000000</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>43308</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>43308</v>
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1500000</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>43308</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>123123</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="O2" s="0" t="n">
         <v>100000</v>
       </c>
-      <c r="N2" s="2" t="n">
-        <v>43308</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>43308</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>17</v>
+      <c r="P2" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,34 +354,39 @@
         <v>1222020</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>150000000</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>43308</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>43308</v>
+        <v>2</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>120000</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>1500000</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>43308</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="N3" s="0" t="n">
         <v>123123</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="O3" s="0" t="n">
         <v>100000</v>
       </c>
-      <c r="N3" s="2" t="n">
-        <v>43308</v>
-      </c>
-      <c r="O3" s="2" t="n">
-        <v>43308</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>17</v>
+      <c r="P3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>43308</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="rbrekke@example.org"/>

</xml_diff>